<commit_message>
Försökt fixa problem med datan, börjat kolla på hur vi kan konstruera mock communities
</commit_message>
<xml_diff>
--- a/Collect sequences/Data/Metadata_sequences.xlsx
+++ b/Collect sequences/Data/Metadata_sequences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claranordquist/Documents/Universitetet/HT24/Tillämpad bioinformatik/Applied-bioinformatics/Collect sequences/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC14A46-2AED-1F4A-8844-0E19121820A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5040FDF3-6E40-064A-A85A-87037E18A2CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{A2038ED0-8F7E-E745-BF2F-2D9FF8201B65}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17040" xr2:uid="{A2038ED0-8F7E-E745-BF2F-2D9FF8201B65}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="Genus in Families" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Metadata" localSheetId="0">Metadata!$A$1:$E$263</definedName>
+    <definedName name="Metadata" localSheetId="0">Metadata!$A$1:$F$263</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{9BCDB5B2-8F92-344C-84F0-44686E13026A}" name="Metadata" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/claranordquist/Documents/Universitetet/HT24/Tillämpad bioinformatik/Applied-bioinformatics/Collect sequences/Test data/Metadata.csv" decimal="," thousands=" ">
+    <textPr sourceFile="/Users/claranordquist/Documents/Universitetet/HT24/Tillämpad bioinformatik/Applied-bioinformatics/Collect sequences/Test data/Metadata.csv" decimal="," thousands=" ">
       <textFields count="5">
         <textField/>
         <textField/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="330">
   <si>
     <t>Abyssisolibacter   </t>
   </si>
@@ -600,9 +600,6 @@
     <t>Sneathia vaginalis </t>
   </si>
   <si>
-    <t>Missing species removed or replaced with their NCBI correspondents</t>
-  </si>
-  <si>
     <t>Candidatus Dwaynesavagella   </t>
   </si>
   <si>
@@ -2532,6 +2529,24 @@
       </rPr>
       <t>LinkOut</t>
     </r>
+  </si>
+  <si>
+    <t>Original list, with heterotypic synonyms</t>
+  </si>
+  <si>
+    <t>Parafannyhessea umbonata</t>
+  </si>
+  <si>
+    <t>Hoylesella timonensis</t>
+  </si>
+  <si>
+    <t>Final list, with missing species replaced with their NCBI correspondents (GTDB-NCBI), or removed</t>
+  </si>
+  <si>
+    <t>Nanoperiomorbus sp004136275*</t>
+  </si>
+  <si>
+    <t>Final list, without families</t>
   </si>
 </sst>
 </file>
@@ -2619,7 +2634,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2628,7 +2643,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2636,9 +2650,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8"/>
@@ -2978,20 +2992,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20183861-4879-2E47-BECC-DE4E5FA6B542}">
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="1" max="4" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>101</v>
       </c>
@@ -2999,11 +3013,16 @@
         <v>102</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>324</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -3013,8 +3032,14 @@
       <c r="C2" s="3" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3024,8 +3049,14 @@
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3035,8 +3066,14 @@
       <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -3046,8 +3083,14 @@
       <c r="C5" s="3" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3057,8 +3100,14 @@
       <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3068,8 +3117,14 @@
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>105</v>
       </c>
@@ -3079,8 +3134,14 @@
       <c r="C8" s="3" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>106</v>
       </c>
@@ -3088,32 +3149,50 @@
         <v>10</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C10" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>108</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C11" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>109</v>
       </c>
@@ -3121,43 +3200,67 @@
         <v>11</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>111</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>113</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>115</v>
       </c>
@@ -3165,10 +3268,16 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -3176,10 +3285,16 @@
         <v>116</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>117</v>
       </c>
@@ -3187,32 +3302,50 @@
         <v>118</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>119</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>121</v>
       </c>
@@ -3220,21 +3353,33 @@
         <v>20</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>122</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>124</v>
       </c>
@@ -3242,32 +3387,50 @@
         <v>25</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>125</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>127</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>128</v>
       </c>
@@ -3275,10 +3438,16 @@
         <v>27</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>129</v>
       </c>
@@ -3286,21 +3455,33 @@
         <v>28</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>130</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>131</v>
       </c>
@@ -3308,21 +3489,33 @@
         <v>32</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>132</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -3330,10 +3523,16 @@
         <v>35</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>133</v>
       </c>
@@ -3341,21 +3540,33 @@
         <v>134</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -3363,10 +3574,16 @@
         <v>46</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -3374,10 +3591,16 @@
         <v>47</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -3385,21 +3608,33 @@
         <v>48</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>34</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -3407,10 +3642,16 @@
         <v>50</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>136</v>
       </c>
@@ -3418,87 +3659,135 @@
         <v>51</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>137</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C42" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>48</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C43" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>49</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>147</v>
+        <v>328</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>50</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C45" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C46" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>140</v>
       </c>
@@ -3506,32 +3795,50 @@
         <v>141</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>57</v>
       </c>
       <c r="B48" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>58</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>144</v>
       </c>
@@ -3539,66 +3846,88 @@
         <v>69</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="12"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>145</v>
       </c>
       <c r="B51" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C51" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E51" s="12"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>147</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" s="12"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C52" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E52" s="12"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>65</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C53" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" s="12"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>148</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C54" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E54" s="13"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>149</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C55" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C55" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>69</v>
       </c>
@@ -3606,10 +3935,13 @@
         <v>75</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>150</v>
       </c>
@@ -3617,10 +3949,13 @@
         <v>76</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>151</v>
       </c>
@@ -3628,66 +3963,82 @@
         <v>152</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>73</v>
       </c>
       <c r="B59" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="C59" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C59" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D59" s="12"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>74</v>
       </c>
       <c r="B60" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C60" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="D60" s="12"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>75</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C61" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D61" s="12"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>156</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C62" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" s="12"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>76</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C63" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D63" s="13"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>157</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="6"/>
+      <c r="C64" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
@@ -3696,7 +4047,9 @@
       <c r="B65" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C65" s="6"/>
+      <c r="C65" s="4" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -3705,7 +4058,9 @@
       <c r="B66" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C66" s="6"/>
+      <c r="C66" s="4" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -3714,7 +4069,9 @@
       <c r="B67" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C67" s="6"/>
+      <c r="C67" s="5" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -3732,8 +4089,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D1:D70">
-    <sortCondition ref="D1:D70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:E54">
+    <sortCondition ref="E54"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3743,8 +4100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0934417-8D6A-0F44-8780-7DA0E5CEB2B0}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3774,7 +4131,7 @@
       <c r="A3" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3782,7 +4139,7 @@
       <c r="A4" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>175</v>
       </c>
     </row>
@@ -3790,7 +4147,7 @@
       <c r="A5" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3798,7 +4155,7 @@
       <c r="A6" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3870,7 +4227,7 @@
       <c r="A15" t="s">
         <v>158</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>178</v>
       </c>
     </row>
@@ -3883,836 +4240,836 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FB95367-E2EB-9047-8AAA-2D9AC4AC46BA}">
   <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28" style="10" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="19.83203125" style="10" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="10"/>
-    <col min="6" max="6" width="21.6640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="26" style="10" customWidth="1"/>
-    <col min="8" max="8" width="24.33203125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="28.5" style="10" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="10" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="28" style="9" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="9" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" style="9" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" style="9"/>
+    <col min="6" max="6" width="21.6640625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="26" style="9" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="28.5" style="9" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="9" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>141</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="F2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="H2" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="10" t="s">
+      <c r="C3" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="G3" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="J3" s="10" t="s">
+      <c r="C4" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="G4" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="J4" s="10" t="s">
+      <c r="C5" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="H5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="J5" s="10" t="s">
+      <c r="C6" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="G6" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J6" s="10" t="s">
+      <c r="C7" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="G7" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="D7" s="10" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>233</v>
-      </c>
-      <c r="I7" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="J7" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="G8" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="10" t="s">
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>236</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>237</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="F11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="I31" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>245</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>304</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="I14" s="11" t="s">
+      <c r="D33" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="I33" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D34" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D35" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="I35" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D36" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="I36" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D37" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I38" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I39" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I40" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I41" s="9" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I42" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I43" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I44" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I45" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I46" s="9" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I47" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I48" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I49" s="9" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I50" s="9" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I51" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I52" s="9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I53" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I54" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I55" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I56" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I57" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I58" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I59" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I60" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I61" s="10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I62" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I63" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I64" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I65" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I66" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I67" s="9" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I68" s="10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I69" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I70" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I71" s="9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I72" s="9" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I73" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I74" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I75" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I76" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I77" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I78" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I79" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I80" s="10" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>306</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>307</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>308</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>309</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>310</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>197</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>312</v>
-      </c>
-      <c r="I23" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="I24" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>314</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>315</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>316</v>
-      </c>
-      <c r="I27" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>319</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>204</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="I31" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="I32" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>321</v>
-      </c>
-      <c r="I33" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D34" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D35" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D36" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="I36" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D37" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I38" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I39" s="11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I40" s="10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I41" s="10" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I42" s="10" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I43" s="11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I44" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I45" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I46" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I47" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I48" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I49" s="10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I50" s="10" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I51" s="10" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I52" s="10" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I53" s="11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I54" s="11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I55" s="10" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I56" s="10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I57" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I58" s="10" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I59" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I60" s="10" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I61" s="11" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I62" s="11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I63" s="10" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I64" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I65" s="10" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I66" s="10" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I67" s="10" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I68" s="11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I69" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I70" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I71" s="10" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I72" s="10" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I73" s="11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I74" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I75" s="11" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I76" s="11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="77" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I77" s="11" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="78" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I78" s="11" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="79" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I79" s="11" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I80" s="11" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>